<commit_message>
changes to power measurements
</commit_message>
<xml_diff>
--- a/powerMeasure/power measurements.xlsx
+++ b/powerMeasure/power measurements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1020" yWindow="460" windowWidth="27780" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>POWER</t>
   </si>
@@ -129,6 +129,51 @@
   </si>
   <si>
     <t>128 byte</t>
+  </si>
+  <si>
+    <t>RECEIVE DATA_OVERHEAR_V</t>
+  </si>
+  <si>
+    <t>RECEIVE DATA_OVERHEAR_TIME</t>
+  </si>
+  <si>
+    <t>3,6 ms</t>
+  </si>
+  <si>
+    <t>196 mV</t>
+  </si>
+  <si>
+    <t>202 mV</t>
+  </si>
+  <si>
+    <t>9 ms</t>
+  </si>
+  <si>
+    <t>216 mV</t>
+  </si>
+  <si>
+    <t>211 mV</t>
+  </si>
+  <si>
+    <t>10,5 ms</t>
+  </si>
+  <si>
+    <t>205 mV</t>
+  </si>
+  <si>
+    <t>Probably only overhear</t>
+  </si>
+  <si>
+    <t>9,4 ms</t>
+  </si>
+  <si>
+    <t>187 mV</t>
+  </si>
+  <si>
+    <t>2,8 V_BATTERY</t>
+  </si>
+  <si>
+    <t>2,7 V_BATTERY</t>
   </si>
 </sst>
 </file>
@@ -152,12 +197,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -172,10 +229,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="191" zoomScalePageLayoutView="191" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,13 +525,15 @@
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -493,29 +555,37 @@
       <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G3" t="s">
@@ -524,93 +594,143 @@
       <c r="H3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="5">
         <v>3.09</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
small changes, in a function
</commit_message>
<xml_diff>
--- a/powerMeasure/power measurements.xlsx
+++ b/powerMeasure/power measurements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="37340" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
   <si>
     <t>POWER</t>
   </si>
@@ -206,9 +206,6 @@
     <t>49 mW</t>
   </si>
   <si>
-    <t>Retransmission flow:</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -255,16 +252,25 @@
   </si>
   <si>
     <t>Retransmits for price of idle 3 sec</t>
+  </si>
+  <si>
+    <t>Retransmission flow with relay:</t>
+  </si>
+  <si>
+    <t>Retransmission flow no relay:</t>
+  </si>
+  <si>
+    <t>Send packet with relay:</t>
+  </si>
+  <si>
+    <t>Send packet no relay:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000E+00"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -280,8 +286,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,8 +352,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE799"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -339,29 +367,151 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -370,6 +520,7 @@
     <mruColors>
       <color rgb="FFF8CCAD"/>
       <color rgb="FFB5C7E7"/>
+      <color rgb="FFFFE799"/>
     </mruColors>
   </colors>
   <extLst>
@@ -643,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,6 +812,7 @@
     <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -855,331 +1007,625 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E17" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+    <row r="25" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8"/>
+      <c r="H26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E27" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="6" t="s">
+      <c r="F27" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="6">
+      <c r="D28" s="13">
         <f>49*10^-3</f>
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="D27" s="6">
+      <c r="E28" s="13">
         <f>10*10^-3</f>
         <v>0.01</v>
       </c>
-      <c r="E27" s="12">
-        <f>C27*D27</f>
+      <c r="F28" s="29">
+        <f>D28*E28</f>
         <v>4.8999999999999998E-4</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="7" t="s">
+      <c r="H28" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I28" s="24">
+        <f>49*10^-3</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J28" s="24">
+        <f t="shared" ref="J28" si="0">10*10^-3</f>
+        <v>0.01</v>
+      </c>
+      <c r="K28" s="25">
+        <f>I28*J28</f>
+        <v>4.8999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="10">
+      <c r="D29" s="15">
         <f>54*10^-3</f>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="D28" s="10">
-        <f t="shared" ref="D28:D38" si="0">10*10^-3</f>
-        <v>0.01</v>
-      </c>
-      <c r="E28" s="13">
-        <f t="shared" ref="E28:E38" si="1">C28*D28</f>
+      <c r="E29" s="15">
+        <f t="shared" ref="E29:E39" si="1">10*10^-3</f>
+        <v>0.01</v>
+      </c>
+      <c r="F29" s="30">
+        <f t="shared" ref="F29:F39" si="2">D29*E29</f>
         <v>5.4000000000000001E-4</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="10">
+      <c r="H29" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I29" s="15">
         <f>54*10^-3</f>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="D29" s="10">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="E29" s="13">
+      <c r="J29" s="15">
+        <f t="shared" ref="J29:J31" si="3">10*10^-3</f>
+        <v>0.01</v>
+      </c>
+      <c r="K29" s="27">
+        <f t="shared" ref="K29:K33" si="4">I29*J29</f>
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="15">
+        <f>54*10^-3</f>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E30" s="15">
         <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="F30" s="30">
+        <f t="shared" si="2"/>
         <v>5.4000000000000001E-4</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="6" t="s">
+      <c r="H30" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" s="15">
+        <f>54*10^-3</f>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J30" s="15">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="K30" s="27">
+        <f t="shared" si="4"/>
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C31" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="6">
+      <c r="D31" s="13">
         <f>49*10^-3</f>
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="D30" s="6">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="E30" s="12">
+      <c r="E31" s="13">
         <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="F31" s="29">
+        <f t="shared" si="2"/>
         <v>4.8999999999999998E-4</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="8" t="s">
+      <c r="H31" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="I31" s="24">
+        <f>49*10^-3</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J31" s="24">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="K31" s="25">
+        <f t="shared" si="4"/>
+        <v>4.8999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C32" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="9">
+      <c r="D32" s="17">
         <f>51*10^-3</f>
         <v>5.1000000000000004E-2</v>
       </c>
-      <c r="D31" s="9">
+      <c r="E32" s="17">
+        <f>3*10^-3</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F32" s="31">
+        <f t="shared" si="2"/>
+        <v>1.5300000000000001E-4</v>
+      </c>
+      <c r="H32" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" s="17">
+        <f>51*10^-3</f>
+        <v>5.1000000000000004E-2</v>
+      </c>
+      <c r="J32" s="17">
+        <f>3*10^-3</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K32" s="37">
+        <f t="shared" si="4"/>
+        <v>1.5300000000000001E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C33" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="15">
+        <f>54*10^-3</f>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E33" s="15">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="F33" s="30">
+        <f t="shared" si="2"/>
+        <v>5.4000000000000001E-4</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" s="15">
+        <f>54*10^-3</f>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J33" s="15">
+        <f t="shared" ref="J33" si="5">10*10^-3</f>
+        <v>0.01</v>
+      </c>
+      <c r="K33" s="27">
+        <f t="shared" si="4"/>
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="13">
+        <f>49*10^-3</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E34" s="13">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="F34" s="29">
+        <f t="shared" si="2"/>
+        <v>4.8999999999999998E-4</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="I34" s="35"/>
+      <c r="J34" s="38">
+        <f>SUM(J28:J33)</f>
+        <v>5.3000000000000005E-2</v>
+      </c>
+      <c r="K34" s="39">
+        <f>SUM(K28:K33)</f>
+        <v>2.7530000000000002E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C35" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="15">
+        <f>54*10^-3</f>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E35" s="15">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="F35" s="30">
+        <f t="shared" si="2"/>
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C36" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="15">
+        <f>54*10^-3</f>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E36" s="15">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="F36" s="30">
+        <f t="shared" si="2"/>
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C37" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="13">
+        <f>49*10^-3</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E37" s="13">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="F37" s="29">
+        <f t="shared" si="2"/>
+        <v>4.8999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C38" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="17">
+        <f>51*10^-3</f>
+        <v>5.1000000000000004E-2</v>
+      </c>
+      <c r="E38" s="17">
         <f>0.3*10^-3</f>
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="E31" s="14">
-        <f t="shared" si="1"/>
+      <c r="F38" s="31">
+        <f t="shared" si="2"/>
         <v>1.5299999999999999E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="10">
+    <row r="39" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C39" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="15">
         <f>54*10^-3</f>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="D32" s="10">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="E32" s="13">
+      <c r="E39" s="15">
         <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="F39" s="30">
+        <f t="shared" si="2"/>
         <v>5.4000000000000001E-4</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="6">
+    <row r="40" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C40" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10">
+        <f>SUM(E28:E39)</f>
+        <v>0.10329999999999998</v>
+      </c>
+      <c r="F40" s="34">
+        <f>SUM(F28:F39)</f>
+        <v>5.3683000000000003E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C41" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="20">
+        <f>51*10^-3</f>
+        <v>5.1000000000000004E-2</v>
+      </c>
+      <c r="E41" s="18">
+        <f>E40</f>
+        <v>0.10329999999999998</v>
+      </c>
+      <c r="F41" s="32">
+        <f>D41*E41</f>
+        <v>5.2682999999999992E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C42" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="32">
+        <f>F40-F41</f>
+        <v>1.0000000000000113E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C43" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="20">
+        <f>51*10^-3</f>
+        <v>5.1000000000000004E-2</v>
+      </c>
+      <c r="E43" s="18">
+        <v>3</v>
+      </c>
+      <c r="F43" s="32">
+        <f>D43*E43</f>
+        <v>0.15300000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="33">
+        <f>F43/F42</f>
+        <v>1529.9999999999829</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C46" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="8"/>
+      <c r="H46" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="8"/>
+    </row>
+    <row r="47" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C47" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K47" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C48" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="24">
         <f>49*10^-3</f>
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="D33" s="6">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="E33" s="12">
-        <f t="shared" si="1"/>
+      <c r="E48" s="13">
+        <f>10*10^-3</f>
+        <v>0.01</v>
+      </c>
+      <c r="F48" s="25">
+        <f>D48*E48</f>
         <v>4.8999999999999998E-4</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="10">
+      <c r="H48" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I48" s="24">
+        <f>49*10^-3</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J48" s="24">
+        <f t="shared" ref="J48:J49" si="6">10*10^-3</f>
+        <v>0.01</v>
+      </c>
+      <c r="K48" s="25">
+        <f>I48*J48</f>
+        <v>4.8999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C49" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" s="15">
         <f>54*10^-3</f>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="D34" s="10">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="E34" s="13">
-        <f t="shared" si="1"/>
+      <c r="E49" s="15">
+        <f t="shared" ref="E49" si="7">10*10^-3</f>
+        <v>0.01</v>
+      </c>
+      <c r="F49" s="27">
+        <f t="shared" ref="F49:F51" si="8">D49*E49</f>
         <v>5.4000000000000001E-4</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" s="10">
+      <c r="H49" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I49" s="15">
         <f>54*10^-3</f>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="D35" s="10">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="E35" s="13">
-        <f t="shared" si="1"/>
+      <c r="J49" s="15">
+        <f t="shared" si="6"/>
+        <v>0.01</v>
+      </c>
+      <c r="K49" s="27">
+        <f>I49*J49</f>
         <v>5.4000000000000001E-4</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="6">
+    <row r="50" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" s="24">
         <f>49*10^-3</f>
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="D36" s="6">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="E36" s="12">
-        <f t="shared" si="1"/>
+      <c r="E50" s="13">
+        <f>10*10^-3</f>
+        <v>0.01</v>
+      </c>
+      <c r="F50" s="25">
+        <f t="shared" si="8"/>
         <v>4.8999999999999998E-4</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="9">
-        <f>51*10^-3</f>
-        <v>5.1000000000000004E-2</v>
-      </c>
-      <c r="D37" s="9">
-        <f>0.3*10^-3</f>
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="E37" s="14">
-        <f t="shared" si="1"/>
-        <v>1.5299999999999999E-5</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="7" t="s">
+      <c r="H50" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22">
+        <f>SUM(J48:J49)</f>
+        <v>0.02</v>
+      </c>
+      <c r="K50" s="40">
+        <f>SUM(K48:K49)</f>
+        <v>1.0300000000000001E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C51" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="10">
+      <c r="D51" s="15">
         <f>54*10^-3</f>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="D38" s="10">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="E38" s="13">
-        <f t="shared" si="1"/>
+      <c r="E51" s="15">
+        <f t="shared" ref="E51" si="9">10*10^-3</f>
+        <v>0.01</v>
+      </c>
+      <c r="F51" s="27">
+        <f t="shared" si="8"/>
         <v>5.4000000000000001E-4</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39">
-        <f>SUM(D27:D38)</f>
-        <v>0.10059999999999998</v>
-      </c>
-      <c r="E39" s="15">
-        <f>SUM(E27:E38)</f>
-        <v>5.2306000000000002E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" s="11">
-        <f>51*10^-3</f>
-        <v>5.1000000000000004E-2</v>
-      </c>
-      <c r="D40">
-        <f>D39</f>
-        <v>0.10059999999999998</v>
-      </c>
-      <c r="E40" s="15">
-        <f>C40*D40</f>
-        <v>5.1305999999999991E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" s="15">
-        <f>E39-E40</f>
-        <v>1.0000000000000113E-4</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="11">
-        <f>51*10^-3</f>
-        <v>5.1000000000000004E-2</v>
-      </c>
-      <c r="D42">
-        <v>3</v>
-      </c>
-      <c r="E42" s="15">
-        <f>C42*D42</f>
-        <v>0.15300000000000002</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>75</v>
-      </c>
-      <c r="E43" s="15">
-        <f>E42/E41</f>
-        <v>1529.9999999999829</v>
+    <row r="52" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35">
+        <f>SUM(E48:E51)</f>
+        <v>0.04</v>
+      </c>
+      <c r="F52" s="36">
+        <f>SUM(F48:F51)</f>
+        <v>2.0600000000000002E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>